<commit_message>
more stuff to do with provisional references / recombinants
</commit_message>
<xml_diff>
--- a/tabular/Missing_NCBI_Refseqs.xlsx
+++ b/tabular/Missing_NCBI_Refseqs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
   <si>
     <t>KJ439769</t>
   </si>
@@ -382,6 +382,75 @@
   </si>
   <si>
     <t>1g</t>
+  </si>
+  <si>
+    <t>Table 4 -- Recombinants</t>
+  </si>
+  <si>
+    <t>RF2k/1b</t>
+  </si>
+  <si>
+    <t>AY587845</t>
+  </si>
+  <si>
+    <t>RF2i/6p</t>
+  </si>
+  <si>
+    <t>3405-3464</t>
+  </si>
+  <si>
+    <t>DQ155560</t>
+  </si>
+  <si>
+    <t>RF2b/1b_1</t>
+  </si>
+  <si>
+    <t>DQ364460</t>
+  </si>
+  <si>
+    <t>RF2/5</t>
+  </si>
+  <si>
+    <t>3366-3389</t>
+  </si>
+  <si>
+    <t>AM408911</t>
+  </si>
+  <si>
+    <t>RF2b/6w</t>
+  </si>
+  <si>
+    <t>EU643835</t>
+  </si>
+  <si>
+    <t>RF2b/1b_2</t>
+  </si>
+  <si>
+    <t>AB622121</t>
+  </si>
+  <si>
+    <t>RF2b/1a</t>
+  </si>
+  <si>
+    <t>3429-3440</t>
+  </si>
+  <si>
+    <t>JF779679</t>
+  </si>
+  <si>
+    <t>RF2b/1b_3</t>
+  </si>
+  <si>
+    <t>3286-3293</t>
+  </si>
+  <si>
+    <t>AB677530</t>
+  </si>
+  <si>
+    <t>RF2b/1b_4</t>
+  </si>
+  <si>
+    <t>AB677527</t>
   </si>
 </sst>
 </file>
@@ -441,8 +510,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -495,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -519,6 +592,8 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -542,6 +617,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -871,13 +948,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q113"/>
+  <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25">
       <c r="A1" s="1" t="s">
@@ -2729,12 +2809,116 @@
         <v>89</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="18">
+    <row r="113" spans="1:3" ht="18">
       <c r="A113" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="18">
+      <c r="A115" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="18">
+      <c r="A116" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B116" s="2">
+        <v>3186</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="18">
+      <c r="A117" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="18">
+      <c r="A118" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" s="2">
+        <v>3456</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="18">
+      <c r="A119" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="18">
+      <c r="A120" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B120" s="2">
+        <v>3429</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="18">
+      <c r="A121" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B121" s="2">
+        <v>3432</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="18">
+      <c r="A122" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="18">
+      <c r="A123" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="18">
+      <c r="A124" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>